<commit_message>
Done with 53. Maximum Subarray without understanding the sol
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaina\Desktop\LeetCode\TwoWeeksStudyPlanToTackleDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaina\Desktop\LeetCode\TwoWeeksStudyPlanToTackleDS\DataStructure1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Solutions</t>
+  </si>
+  <si>
+    <t>Understanding</t>
+  </si>
+  <si>
+    <t>No sol given and didn't understood provided sol</t>
+  </si>
+  <si>
+    <t>Given 1 sol and understood the other 2</t>
   </si>
 </sst>
 </file>
@@ -431,20 +443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,10 +474,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>217</v>
       </c>
@@ -480,11 +499,17 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>53</v>
       </c>
@@ -497,11 +522,14 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -513,6 +541,9 @@
       </c>
       <c r="E4" t="s">
         <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with 1. Two Sum
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>No.</t>
   </si>
@@ -80,7 +80,10 @@
     <t>No sol given and didn't understood provided sol</t>
   </si>
   <si>
-    <t>Given 1 sol and understood the other 2</t>
+    <t>Given O(n^2) sol and understood the other 2</t>
+  </si>
+  <si>
+    <t>Dict, enumerate function</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,6 +525,9 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
@@ -539,10 +545,34 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done with 88. Merge Sorted Array
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>No.</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>Dict, enumerate function</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Merge sort</t>
+  </si>
+  <si>
+    <t>Given O(nlogn) sol and didn't understood the merge sort sol</t>
+  </si>
+  <si>
+    <t>0% understanding</t>
+  </si>
+  <si>
+    <t>50% understanding</t>
+  </si>
+  <si>
+    <t>100% understanding</t>
   </si>
 </sst>
 </file>
@@ -120,7 +138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +148,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,11 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +526,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>217</v>
       </c>
       <c r="B2" t="s">
@@ -513,7 +552,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>53</v>
       </c>
       <c r="B3" t="s">
@@ -536,7 +575,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -562,8 +601,29 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
-        <v>13</v>
+      <c r="A5" s="6">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -574,6 +634,24 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G7" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+      <c r="I18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="4"/>
+      <c r="I20" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with 350. Intersection of Two Arrays II
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>No.</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
     <t>Contain Duplicates</t>
   </si>
   <si>
@@ -102,6 +99,36 @@
   </si>
   <si>
     <t>100% understanding</t>
+  </si>
+  <si>
+    <t>Main Topic</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Array, Hash table, Sorting</t>
+  </si>
+  <si>
+    <t>Array, Divide and conquer</t>
+  </si>
+  <si>
+    <t>Array, Hash table</t>
+  </si>
+  <si>
+    <t>Array, two pointers, sorting</t>
+  </si>
+  <si>
+    <t>Array, Hash table, two pointers</t>
+  </si>
+  <si>
+    <t>Intersection of two arrays 2</t>
+  </si>
+  <si>
+    <t>Dict</t>
+  </si>
+  <si>
+    <t>Given O(n^2) and O(n) sol</t>
   </si>
 </sst>
 </file>
@@ -197,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -205,6 +232,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,21 +527,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,151 +550,190 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>217</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>88</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>350</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="9"/>
+      <c r="J18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="5"/>
-      <c r="I18" t="s">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="10"/>
+      <c r="J19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="6"/>
-      <c r="I19" t="s">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="11"/>
+      <c r="J20" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="4"/>
-      <c r="I20" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with 121. Best Time to Buy and Sell Stock
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>No.</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>Given O(n^2) and O(n) sol</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Array, Dynamic Prog</t>
+  </si>
+  <si>
+    <t>Given O(n) sol but not accepted hence sol by chatGPT without understanding</t>
   </si>
 </sst>
 </file>
@@ -530,7 +539,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,8 +722,74 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" s="3" t="s">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done with 566. Reshape the matrix
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>No.</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Given O(n) sol but not accepted hence sol by chatGPT without understanding</t>
+  </si>
+  <si>
+    <t>Reshape the matrix</t>
+  </si>
+  <si>
+    <t>Array, Matrix, Simulation</t>
+  </si>
+  <si>
+    <t>Given O(n^2) sol and didn't see any other sol</t>
   </si>
 </sst>
 </file>
@@ -539,7 +548,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,9 +757,30 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="3" t="s">
-        <v>12</v>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>566</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 118. Pascals triangle
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>No.</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Given O(n^2) sol and didn't see any other sol</t>
+  </si>
+  <si>
+    <t>Pascal's triangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array </t>
+  </si>
+  <si>
+    <t>Copied from Solution pane and didn't understand</t>
   </si>
 </sst>
 </file>
@@ -548,7 +557,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,9 +792,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="3" t="s">
-        <v>12</v>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 74. Search a 2D matrix
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>No.</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Copied from Solution pane and didn't understand</t>
+  </si>
+  <si>
+    <t>Search a 2D matrix</t>
+  </si>
+  <si>
+    <t>Array, Hash table, matrix</t>
   </si>
 </sst>
 </file>
@@ -556,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,9 +824,30 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H10" s="3" t="s">
-        <v>12</v>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 36. Valid Sudoku
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>No.</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Array, Hash table, matrix</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>Array, Binary search, matrix</t>
   </si>
 </sst>
 </file>
@@ -562,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>118</v>
       </c>
@@ -824,7 +830,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>74</v>
       </c>
@@ -835,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -850,9 +856,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H11" s="3" t="s">
-        <v>12</v>
+    <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 387. First Unique Character in a String
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>No.</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>Array, Binary search, matrix</t>
+  </si>
+  <si>
+    <t>First Unique Character in a String</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>String, Hash table, Queue</t>
+  </si>
+  <si>
+    <t>Given 2 solutions. 1 O(n^2) and 2nd O(n). Havent seen solution pane</t>
   </si>
 </sst>
 </file>
@@ -568,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,9 +894,33 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="3" t="s">
-        <v>12</v>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>387</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 242. Valid Inagram
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>No.</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>Given 2 solutions. 1 O(n^2) and 2nd O(n). Havent seen solution pane</t>
+  </si>
+  <si>
+    <t>Valid Inagram</t>
+  </si>
+  <si>
+    <t>String, Hash table, Sorting</t>
+  </si>
+  <si>
+    <t>Given 1 solution and copied 1 from solutions</t>
   </si>
 </sst>
 </file>
@@ -580,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,9 +932,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="3" t="s">
-        <v>12</v>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>242</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 383. Ransom note
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>No.</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>Given 1 solution and copied 1 from solutions</t>
+  </si>
+  <si>
+    <t>Ransome Note</t>
+  </si>
+  <si>
+    <t>String, Hash table, Counting</t>
+  </si>
+  <si>
+    <t>Given O(n) sol and didn't see any other sol</t>
   </si>
 </sst>
 </file>
@@ -590,7 +599,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,9 +970,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="3" t="s">
-        <v>12</v>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>383</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started SQL Study plan i.e. SQL 1
</commit_message>
<xml_diff>
--- a/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
+++ b/TwoWeeksStudyPlanToTackleDS/DataStructure1/ProbList.xlsx
@@ -598,20 +598,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="8" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>